<commit_message>
added the multi injection
</commit_message>
<xml_diff>
--- a/template3.xlsx
+++ b/template3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20148" windowHeight="7955"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3403,8 +3403,8 @@
   <sheetPr/>
   <dimension ref="A1:AB1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:K2"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15" customHeight="1"/>

</xml_diff>